<commit_message>
MANUAL CLEAN convo minor edits [wiki examples dataset]
</commit_message>
<xml_diff>
--- a/src/SpeakSingapore/data/wiki_examples_ERG/processed_step_3_manual_label/processed_step_3_manual_clean_convo.xlsx
+++ b/src/SpeakSingapore/data/wiki_examples_ERG/processed_step_3_manual_label/processed_step_3_manual_clean_convo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pongyizhen/Desktop/Github/SpeakSingapore/src/SpeakSingapore/data/wiki_examples_ERG/processed_step_3_manual_label/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D6CD3B-4847-9845-88C7-5F293CAF72B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E921D2-DA30-6F48-B228-744E131F4588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>original_sentence</t>
   </si>
@@ -212,16 +212,10 @@
 Student A: Thank you</t>
   </si>
   <si>
-    <t>yz_label</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 A: Aiyo, nearly hit me leh, so scary sia
 B: Alamak, why he drive so fast?
 A: Ya, dangerous sia</t>
-  </si>
-  <si>
-    <t>hy_label</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -705,7 +699,7 @@
         <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -713,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -728,10 +722,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -740,7 +734,7 @@
     <col min="5" max="5" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -754,16 +748,10 @@
         <v>30</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -777,10 +765,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -788,16 +776,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -805,16 +793,16 @@
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -822,16 +810,16 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="208" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -839,16 +827,16 @@
         <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -856,16 +844,16 @@
         <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="176" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -879,10 +867,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -896,10 +884,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -907,16 +895,16 @@
         <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -924,16 +912,16 @@
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -941,16 +929,16 @@
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -958,16 +946,16 @@
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -981,10 +969,10 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -998,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>